<commit_message>
Creating a real json format with all the content inside
</commit_message>
<xml_diff>
--- a/data/Spain1.xlsx
+++ b/data/Spain1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirk3n/Desktop/nuts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirk3n/Documents/Programacion/nuts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB08CEC7-FE10-BA43-8D18-536AEE7A9F25}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEC1156-2EC3-2647-A6C7-63C6B189ADC7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>List of schools participating in the programme</t>
   </si>
@@ -96,6 +95,15 @@
   </si>
   <si>
     <t>SPAIN4</t>
+  </si>
+  <si>
+    <t>SPAIN5</t>
+  </si>
+  <si>
+    <t>Colegio Cristo Reyasd42345234563425345</t>
+  </si>
+  <si>
+    <t>ES301</t>
   </si>
 </sst>
 </file>
@@ -645,7 +653,7 @@
   <dimension ref="A1:I999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -753,11 +761,21 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -2350,9 +2368,10 @@
     <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{A50F83D1-F666-6F45-A742-C67991B4B640}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{1986FEDD-3374-BF4D-A874-DEDFDC6BCE28}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{3204EFB0-7D82-E544-B380-34A41CF380D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Including restrinctions of the NUTs (300, 30)
</commit_message>
<xml_diff>
--- a/data/Spain1.xlsx
+++ b/data/Spain1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirk3n/Documents/Programacion/nuts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEC1156-2EC3-2647-A6C7-63C6B189ADC7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9540512-FA53-3C4D-81EF-C41DA503D5FC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>List of schools participating in the programme</t>
   </si>
@@ -103,7 +103,13 @@
     <t>Colegio Cristo Reyasd42345234563425345</t>
   </si>
   <si>
-    <t>ES301</t>
+    <t>ES13</t>
+  </si>
+  <si>
+    <t>Mierda frita</t>
+  </si>
+  <si>
+    <t>ES412</t>
   </si>
 </sst>
 </file>
@@ -653,7 +659,7 @@
   <dimension ref="A1:I999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -778,11 +784,21 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -2369,9 +2385,10 @@
     <hyperlink ref="D5" r:id="rId2" xr:uid="{A50F83D1-F666-6F45-A742-C67991B4B640}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{1986FEDD-3374-BF4D-A874-DEDFDC6BCE28}"/>
     <hyperlink ref="D7" r:id="rId4" xr:uid="{3204EFB0-7D82-E544-B380-34A41CF380D2}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{D645B445-E63A-B84C-B7FC-FAE76E995DA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>